<commit_message>
Continue visualisation course + PP dashboard
</commit_message>
<xml_diff>
--- a/Dummy data (3 months).xlsx
+++ b/Dummy data (3 months).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalieheng/Desktop/Private/My Projects/Project 1 - Purchases and Transaction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F7E370-AB78-3442-B9EB-464EBE182DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1BAFE6-C579-104E-B685-B75143B048B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{303B41FA-64CF-E341-99BD-C3699F8D67DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t xml:space="preserve">Price </t>
+  </si>
+  <si>
+    <t>Total Inflow</t>
+  </si>
+  <si>
+    <t>Total Budget</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596455D4-6055-9C49-9E0F-4AD845AC3010}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,7 +491,7 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +504,14 @@
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>44562</v>
       </c>
@@ -512,8 +524,14 @@
       <c r="D2" s="4">
         <v>45.67</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>44563</v>
       </c>
@@ -526,8 +544,14 @@
       <c r="D3" s="4">
         <v>35.119999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>44564</v>
       </c>
@@ -540,8 +564,14 @@
       <c r="D4" s="4">
         <v>8.99</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>44565</v>
       </c>
@@ -554,8 +584,14 @@
       <c r="D5" s="4">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>44566</v>
       </c>
@@ -568,8 +604,14 @@
       <c r="D6" s="4">
         <v>67.89</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>44567</v>
       </c>
@@ -582,8 +624,14 @@
       <c r="D7" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>44568</v>
       </c>
@@ -596,8 +644,14 @@
       <c r="D8" s="4">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>44569</v>
       </c>
@@ -610,8 +664,14 @@
       <c r="D9" s="4">
         <v>112.45</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>44570</v>
       </c>
@@ -624,8 +684,14 @@
       <c r="D10" s="4">
         <v>23.12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>44571</v>
       </c>
@@ -638,8 +704,14 @@
       <c r="D11" s="4">
         <v>40.229999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>44572</v>
       </c>
@@ -652,8 +724,14 @@
       <c r="D12" s="4">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>44573</v>
       </c>
@@ -666,8 +744,14 @@
       <c r="D13" s="4">
         <v>28.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>44574</v>
       </c>
@@ -680,8 +764,14 @@
       <c r="D14" s="4">
         <v>45.67</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>44575</v>
       </c>
@@ -694,8 +784,14 @@
       <c r="D15" s="4">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>44576</v>
       </c>
@@ -708,8 +804,14 @@
       <c r="D16" s="4">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>44577</v>
       </c>
@@ -722,8 +824,14 @@
       <c r="D17" s="4">
         <v>89.99</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>44578</v>
       </c>
@@ -736,8 +844,14 @@
       <c r="D18" s="4">
         <v>41.23</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>44579</v>
       </c>
@@ -750,8 +864,14 @@
       <c r="D19" s="4">
         <v>37.119999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>44580</v>
       </c>
@@ -764,8 +884,14 @@
       <c r="D20" s="4">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>44581</v>
       </c>
@@ -778,8 +904,14 @@
       <c r="D21" s="4">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>44582</v>
       </c>
@@ -792,8 +924,14 @@
       <c r="D22" s="4">
         <v>78.900000000000006</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>44583</v>
       </c>
@@ -806,8 +944,14 @@
       <c r="D23" s="4">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>44584</v>
       </c>
@@ -820,8 +964,14 @@
       <c r="D24" s="4">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>44585</v>
       </c>
@@ -834,8 +984,14 @@
       <c r="D25" s="4">
         <v>102.45</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>44586</v>
       </c>
@@ -848,8 +1004,14 @@
       <c r="D26" s="4">
         <v>27.23</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>44587</v>
       </c>
@@ -862,8 +1024,14 @@
       <c r="D27" s="4">
         <v>38.229999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>44588</v>
       </c>
@@ -876,8 +1044,14 @@
       <c r="D28" s="4">
         <v>10.99</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>44589</v>
       </c>
@@ -890,8 +1064,14 @@
       <c r="D29" s="4">
         <v>26.75</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>44590</v>
       </c>
@@ -904,8 +1084,14 @@
       <c r="D30" s="4">
         <v>55.67</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>44591</v>
       </c>
@@ -918,8 +1104,14 @@
       <c r="D31" s="4">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>44593</v>
       </c>
@@ -932,8 +1124,14 @@
       <c r="D32" s="4">
         <v>42.89</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>44594</v>
       </c>
@@ -946,8 +1144,14 @@
       <c r="D33" s="4">
         <v>30.12</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>44595</v>
       </c>
@@ -960,8 +1164,14 @@
       <c r="D34" s="4">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>44596</v>
       </c>
@@ -974,8 +1184,14 @@
       <c r="D35" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>44597</v>
       </c>
@@ -988,8 +1204,14 @@
       <c r="D36" s="4">
         <v>68.989999999999995</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>44598</v>
       </c>
@@ -1002,8 +1224,14 @@
       <c r="D37" s="4">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>44599</v>
       </c>
@@ -1016,8 +1244,14 @@
       <c r="D38" s="4">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>44600</v>
       </c>
@@ -1030,8 +1264,14 @@
       <c r="D39" s="4">
         <v>110.45</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>44601</v>
       </c>
@@ -1044,8 +1284,14 @@
       <c r="D40" s="4">
         <v>23.56</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44602</v>
       </c>
@@ -1058,8 +1304,14 @@
       <c r="D41" s="4">
         <v>40.229999999999997</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>44603</v>
       </c>
@@ -1072,8 +1324,14 @@
       <c r="D42" s="4">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>44604</v>
       </c>
@@ -1086,8 +1344,14 @@
       <c r="D43" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>44605</v>
       </c>
@@ -1100,8 +1364,14 @@
       <c r="D44" s="4">
         <v>46.67</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44606</v>
       </c>
@@ -1114,8 +1384,14 @@
       <c r="D45" s="4">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>44607</v>
       </c>
@@ -1128,8 +1404,14 @@
       <c r="D46" s="4">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>44608</v>
       </c>
@@ -1142,8 +1424,14 @@
       <c r="D47" s="4">
         <v>89.99</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>44609</v>
       </c>
@@ -1156,8 +1444,14 @@
       <c r="D48" s="4">
         <v>37.229999999999997</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>44610</v>
       </c>
@@ -1170,8 +1464,14 @@
       <c r="D49" s="4">
         <v>35.119999999999997</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>44611</v>
       </c>
@@ -1184,8 +1484,14 @@
       <c r="D50" s="4">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>44612</v>
       </c>
@@ -1198,8 +1504,14 @@
       <c r="D51" s="4">
         <v>22.75</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F51" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>44613</v>
       </c>
@@ -1212,8 +1524,14 @@
       <c r="D52" s="4">
         <v>49.99</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>44614</v>
       </c>
@@ -1226,8 +1544,14 @@
       <c r="D53" s="4">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>44615</v>
       </c>
@@ -1240,8 +1564,14 @@
       <c r="D54" s="4">
         <v>85</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>44616</v>
       </c>
@@ -1254,8 +1584,14 @@
       <c r="D55" s="4">
         <v>102.45</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>44617</v>
       </c>
@@ -1268,8 +1604,14 @@
       <c r="D56" s="4">
         <v>29.23</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>44618</v>
       </c>
@@ -1282,8 +1624,14 @@
       <c r="D57" s="4">
         <v>38.229999999999997</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>44619</v>
       </c>
@@ -1296,8 +1644,14 @@
       <c r="D58" s="4">
         <v>10.99</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>44620</v>
       </c>
@@ -1310,8 +1664,14 @@
       <c r="D59" s="4">
         <v>26.75</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>44621</v>
       </c>
@@ -1324,8 +1684,14 @@
       <c r="D60" s="4">
         <v>35.67</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F60" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>44622</v>
       </c>
@@ -1338,8 +1704,14 @@
       <c r="D61" s="4">
         <v>25.42</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>44623</v>
       </c>
@@ -1352,8 +1724,14 @@
       <c r="D62" s="4">
         <v>7.99</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>44624</v>
       </c>
@@ -1366,8 +1744,14 @@
       <c r="D63" s="4">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>44625</v>
       </c>
@@ -1380,8 +1764,14 @@
       <c r="D64" s="4">
         <v>56.78</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>44626</v>
       </c>
@@ -1394,8 +1784,14 @@
       <c r="D65" s="4">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>44627</v>
       </c>
@@ -1408,8 +1804,14 @@
       <c r="D66" s="4">
         <v>85</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>44628</v>
       </c>
@@ -1422,8 +1824,14 @@
       <c r="D67" s="4">
         <v>99.95</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>44629</v>
       </c>
@@ -1436,8 +1844,14 @@
       <c r="D68" s="4">
         <v>28.34</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>44630</v>
       </c>
@@ -1450,8 +1864,14 @@
       <c r="D69" s="4">
         <v>36.119999999999997</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>44631</v>
       </c>
@@ -1464,8 +1884,14 @@
       <c r="D70" s="4">
         <v>10.99</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>44632</v>
       </c>
@@ -1478,8 +1904,14 @@
       <c r="D71" s="4">
         <v>23.75</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>44633</v>
       </c>
@@ -1492,8 +1924,14 @@
       <c r="D72" s="4">
         <v>45.99</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>44634</v>
       </c>
@@ -1506,8 +1944,14 @@
       <c r="D73" s="4">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>44635</v>
       </c>
@@ -1520,8 +1964,14 @@
       <c r="D74" s="4">
         <v>90</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F74" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>44636</v>
       </c>
@@ -1534,8 +1984,14 @@
       <c r="D75" s="4">
         <v>110.45</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>44637</v>
       </c>
@@ -1548,8 +2004,14 @@
       <c r="D76" s="4">
         <v>31.23</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F76" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>44638</v>
       </c>
@@ -1562,8 +2024,14 @@
       <c r="D77" s="4">
         <v>29.45</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F77" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>44639</v>
       </c>
@@ -1576,8 +2044,14 @@
       <c r="D78" s="4">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F78" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>44640</v>
       </c>
@@ -1590,8 +2064,14 @@
       <c r="D79" s="4">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>44641</v>
       </c>
@@ -1604,8 +2084,14 @@
       <c r="D80" s="4">
         <v>62.99</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F80" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>44642</v>
       </c>
@@ -1618,8 +2104,14 @@
       <c r="D81" s="4">
         <v>68</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>44643</v>
       </c>
@@ -1632,8 +2124,14 @@
       <c r="D82" s="4">
         <v>95</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>44644</v>
       </c>
@@ -1646,8 +2144,14 @@
       <c r="D83" s="4">
         <v>112.99</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>44645</v>
       </c>
@@ -1660,8 +2164,14 @@
       <c r="D84" s="4">
         <v>26.23</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>44646</v>
       </c>
@@ -1674,8 +2184,14 @@
       <c r="D85" s="4">
         <v>39.56</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>44647</v>
       </c>
@@ -1688,8 +2204,14 @@
       <c r="D86" s="4">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>44648</v>
       </c>
@@ -1702,8 +2224,14 @@
       <c r="D87" s="4">
         <v>21.75</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>44649</v>
       </c>
@@ -1716,8 +2244,14 @@
       <c r="D88" s="4">
         <v>36.99</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>44650</v>
       </c>
@@ -1729,6 +2263,12 @@
       </c>
       <c r="D89" s="4">
         <v>80</v>
+      </c>
+      <c r="E89" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>